<commit_message>
adiconando verificação de exceções
</commit_message>
<xml_diff>
--- a/gastos.xlsx
+++ b/gastos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor Lucas\Desktop\Desafio Stone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57B7785-7210-4708-867D-FDFEB1036975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E64ECD-9695-4C43-B099-7D13C0AE9100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13620" yWindow="-120" windowWidth="13740" windowHeight="21240" xr2:uid="{E9E6E8B4-9C39-40B8-8260-1EDE6095F66A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9E6E8B4-9C39-40B8-8260-1EDE6095F66A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>